<commit_message>
Framework, Class, Basepage update
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/LMSData.xlsx
+++ b/src/test/resources/testData/LMSData.xlsx
@@ -1,17 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Febi\NumpyNinja\Hackathon\LMS_UI_Hackathon_Oct24\Team4_SeleniumSquad_LMSUI\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468567F4-6279-401E-9E46-CA8D34C15BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Class" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>testcase</t>
   </si>
@@ -38,21 +61,71 @@
   </si>
   <si>
     <t>hgjhgjh</t>
+  </si>
+  <si>
+    <t>Batchname</t>
+  </si>
+  <si>
+    <t>ClassTopic</t>
+  </si>
+  <si>
+    <t>ClassDescription</t>
+  </si>
+  <si>
+    <t>SelectClassDates</t>
+  </si>
+  <si>
+    <t>NoofClasses</t>
+  </si>
+  <si>
+    <t>StaffName</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Recording</t>
+  </si>
+  <si>
+    <t>validInputAll</t>
+  </si>
+  <si>
+    <t>validInputMandatory</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>Oracle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -62,36 +135,46 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -281,23 +364,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.25"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -308,18 +396,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -331,6 +419,77 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{C029B5E5-F3C9-4D25-B852-132970CAF380}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B4F31D4-4607-44BA-AE04-13824B74BD83}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Febi branch merge (#9)
* Framework, Class, Basepage update

* Singleton and Page Factory update

* git ignore

* Update WebDriverFactory.java

---------

Co-authored-by: sdetninjas <judefebi@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/LMSData.xlsx
+++ b/src/test/resources/testData/LMSData.xlsx
@@ -1,17 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Febi\NumpyNinja\Hackathon\LMS_UI_Hackathon_Oct24\Team4_SeleniumSquad_LMSUI\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468567F4-6279-401E-9E46-CA8D34C15BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Login" sheetId="1" r:id="rId4"/>
+    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Class" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>testcase</t>
   </si>
@@ -38,21 +61,71 @@
   </si>
   <si>
     <t>hgjhgjh</t>
+  </si>
+  <si>
+    <t>Batchname</t>
+  </si>
+  <si>
+    <t>ClassTopic</t>
+  </si>
+  <si>
+    <t>ClassDescription</t>
+  </si>
+  <si>
+    <t>SelectClassDates</t>
+  </si>
+  <si>
+    <t>NoofClasses</t>
+  </si>
+  <si>
+    <t>StaffName</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Recording</t>
+  </si>
+  <si>
+    <t>validInputAll</t>
+  </si>
+  <si>
+    <t>validInputMandatory</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>Oracle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -62,36 +135,46 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -281,23 +364,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.25"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -308,18 +396,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -331,6 +419,77 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{C029B5E5-F3C9-4D25-B852-132970CAF380}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B4F31D4-4607-44BA-AE04-13824B74BD83}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Class Module update
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/LMSData.xlsx
+++ b/src/test/resources/testData/LMSData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Febi\NumpyNinja\Hackathon\LMS_UI_Hackathon_Oct24\Team4_SeleniumSquad_LMSUI\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468567F4-6279-401E-9E46-CA8D34C15BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA36F2A-B559-4B53-8DF2-C845187ADA1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>testcase</t>
   </si>
@@ -99,17 +99,59 @@
     <t>validInputMandatory</t>
   </si>
   <si>
-    <t>Invalid</t>
-  </si>
-  <si>
-    <t>Oracle</t>
+    <t>11/26/2024,11/27/2024</t>
+  </si>
+  <si>
+    <t>Urmila Rao</t>
+  </si>
+  <si>
+    <t>Micro service-01</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>API01</t>
+  </si>
+  <si>
+    <t>InvalidInputMandatory</t>
+  </si>
+  <si>
+    <t>ExpectedMsg</t>
+  </si>
+  <si>
+    <t>Successful</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Postman</t>
+  </si>
+  <si>
+    <t>11/20/2024, 11/22/2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postman API </t>
+  </si>
+  <si>
+    <t>Postman Classes</t>
+  </si>
+  <si>
+    <t>Install Postamn tool</t>
+  </si>
+  <si>
+    <t>zoom</t>
+  </si>
+  <si>
+    <t>SMPO-0001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -127,6 +169,13 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -151,10 +200,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -428,15 +479,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B4F31D4-4607-44BA-AE04-13824B74BD83}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +500,7 @@
       <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E1" t="s">
@@ -461,32 +515,89 @@
       <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3">
+        <v>45209</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
keeping only positive flow
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/LMSData.xlsx
+++ b/src/test/resources/testData/LMSData.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>testcase</t>
   </si>
@@ -93,38 +93,86 @@
     <t>ProgramStatus</t>
   </si>
   <si>
-    <t>MSFinance</t>
+    <t>ValidInputAllOne</t>
+  </si>
+  <si>
+    <t>poland</t>
+  </si>
+  <si>
+    <t>for other modules</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>ValidInputAllTwo</t>
+  </si>
+  <si>
+    <t>africa</t>
+  </si>
+  <si>
+    <t>to edit and delete</t>
+  </si>
+  <si>
+    <t>ValidInputThree</t>
+  </si>
+  <si>
+    <t>australia</t>
+  </si>
+  <si>
+    <t>multi delete</t>
+  </si>
+  <si>
+    <t>ValidInputFour</t>
+  </si>
+  <si>
+    <t>canada</t>
+  </si>
+  <si>
+    <t>extra one</t>
+  </si>
+  <si>
+    <t>BlankProgramName</t>
   </si>
   <si>
     <t>undergrad</t>
   </si>
   <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>BlankProgramName</t>
-  </si>
-  <si>
-    <t>inactive</t>
-  </si>
-  <si>
     <t>InvalidProgramName</t>
   </si>
   <si>
-    <t>MSFinance-</t>
+    <t>a</t>
   </si>
   <si>
     <t>BlankDescriptionName</t>
   </si>
   <si>
+    <t>randomName</t>
+  </si>
+  <si>
     <t>BlankStatus</t>
+  </si>
+  <si>
+    <t>EditProgramNameOnly</t>
+  </si>
+  <si>
+    <t>aaaaEdited</t>
+  </si>
+  <si>
+    <t>EditProgramDescOnly</t>
+  </si>
+  <si>
+    <t>knjjkd edited</t>
+  </si>
+  <si>
+    <t>EditProgramStatusOnly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -147,13 +195,23 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -162,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -171,6 +229,9 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2542,64 +2603,130 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>19</v>
+      <c r="A2" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>40</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated batch test data
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/LMSData.xlsx
+++ b/src/test/resources/testData/LMSData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Febi\NumpyNinja\Hackathon\LMS_UI_Hackathon_Oct24\Team4_SeleniumSquad_LMSUI\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prasaddige/git/Team4_SeleniumSquad_LMSUI/src/test/resources/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CE840C-6CC1-4CAF-A46F-A22E893BF79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810544D6-497A-4340-AFC8-D56370158921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Class" sheetId="2" r:id="rId2"/>
+    <sheet name="Batch" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
   <si>
     <t>testcase</t>
   </si>
@@ -148,6 +148,90 @@
   </si>
   <si>
     <t>class</t>
+  </si>
+  <si>
+    <t>ProgramName</t>
+  </si>
+  <si>
+    <t>BatchNamePrefix</t>
+  </si>
+  <si>
+    <t>BatchName</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>NumberOfClasses</t>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+  </si>
+  <si>
+    <t>My Test Batch</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>InvalidBatchName</t>
+  </si>
+  <si>
+    <t>aaaa</t>
+  </si>
+  <si>
+    <t>ValidProgramName</t>
+  </si>
+  <si>
+    <t>InvalidBatchNamePrefix</t>
+  </si>
+  <si>
+    <t>MissingProgram</t>
+  </si>
+  <si>
+    <t>Program Name is required.</t>
+  </si>
+  <si>
+    <t>MissingBatchName</t>
+  </si>
+  <si>
+    <t>Batch Name is required.</t>
+  </si>
+  <si>
+    <t>MissingStatus</t>
+  </si>
+  <si>
+    <t>Status is required.</t>
+  </si>
+  <si>
+    <t>MissingDesc</t>
+  </si>
+  <si>
+    <t>Batch Description is required.</t>
+  </si>
+  <si>
+    <t>MissingNoOfClass</t>
+  </si>
+  <si>
+    <t>Number of classes is required.</t>
+  </si>
+  <si>
+    <t>InvalidDescriptionEdit</t>
+  </si>
+  <si>
+    <t>This field should start with an alphabet and min 2 character.</t>
+  </si>
+  <si>
+    <t>ValidEdit</t>
+  </si>
+  <si>
+    <t>ValidSearch</t>
+  </si>
+  <si>
+    <t>TeamFourSDETThree</t>
+  </si>
+  <si>
+    <t>TeamFourSDETThree1234</t>
   </si>
 </sst>
 </file>
@@ -165,6 +249,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -172,6 +257,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -203,12 +289,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -434,12 +523,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -461,7 +550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -478,16 +567,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B4F31D4-4607-44BA-AE04-13824B74BD83}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,7 +614,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -545,7 +634,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -577,7 +666,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
@@ -597,7 +686,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>35</v>
       </c>
@@ -612,6 +701,257 @@
       </c>
       <c r="K5" s="4" t="s">
         <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60644E1D-B456-124C-A5C4-6947EE9E01A8}">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" customWidth="1"/>
+    <col min="8" max="8" width="41.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3">
+        <v>1234</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6">
+        <v>1212</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="D7">
+        <v>1212</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9">
+        <v>1212</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10">
+        <v>1212</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11">
+        <v>1212</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12">
+        <v>1123</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>